<commit_message>
soil moisture bugs fixed
</commit_message>
<xml_diff>
--- a/waterbudget from Historic for Maria.xlsx
+++ b/waterbudget from Historic for Maria.xlsx
@@ -449,6 +449,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -457,9 +460,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -898,11 +898,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="87785856"/>
-        <c:axId val="87787392"/>
+        <c:axId val="95379456"/>
+        <c:axId val="95380992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87785856"/>
+        <c:axId val="95379456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +911,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87787392"/>
+        <c:crossAx val="95380992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -919,7 +919,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87787392"/>
+        <c:axId val="95380992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87785856"/>
+        <c:crossAx val="95379456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1372,11 +1372,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="67256320"/>
-        <c:axId val="67257856"/>
+        <c:axId val="95411584"/>
+        <c:axId val="95491200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67256320"/>
+        <c:axId val="95411584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,7 +1385,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67257856"/>
+        <c:crossAx val="95491200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1393,7 +1393,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67257856"/>
+        <c:axId val="95491200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,7 +1404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67256320"/>
+        <c:crossAx val="95411584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1667,11 +1667,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="87840256"/>
-        <c:axId val="87841792"/>
+        <c:axId val="95513984"/>
+        <c:axId val="96334976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87840256"/>
+        <c:axId val="95513984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,7 +1680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87841792"/>
+        <c:crossAx val="96334976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1688,7 +1688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87841792"/>
+        <c:axId val="96334976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1699,7 +1699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87840256"/>
+        <c:crossAx val="95513984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7639,10 +7639,10 @@
   <dimension ref="A1:Q690"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H30" sqref="H30:H31"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7694,21 +7694,21 @@
       <c r="B5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23" t="s">
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
@@ -7905,47 +7905,47 @@
       </c>
       <c r="B13" s="16">
         <f>F13-C13</f>
-        <v>47.771999999999991</v>
+        <v>35.007000000000005</v>
       </c>
       <c r="C13" s="16">
         <f>SUM(C14:C15)</f>
-        <v>24.428000000000001</v>
+        <v>15.7</v>
       </c>
       <c r="D13" s="16">
         <f>SUM(D14:D15)</f>
-        <v>52.195</v>
+        <v>37.26</v>
       </c>
       <c r="E13" s="16">
         <f>C13-D13</f>
-        <v>-27.766999999999999</v>
+        <v>-21.56</v>
       </c>
       <c r="F13" s="16">
         <f>SUM(F14:F15)</f>
-        <v>72.199999999999989</v>
+        <v>50.707000000000001</v>
       </c>
       <c r="G13" s="16">
         <f>SUM(G14:G15)</f>
-        <v>44.5</v>
+        <v>16.579999999999998</v>
       </c>
       <c r="H13" s="16">
         <f>F13-G13</f>
-        <v>27.699999999999989</v>
+        <v>34.127000000000002</v>
       </c>
       <c r="I13" s="16">
         <f>SUM(C13,F13)</f>
-        <v>96.627999999999986</v>
+        <v>66.406999999999996</v>
       </c>
       <c r="J13" s="16">
         <f t="shared" ref="J13:J15" si="0">SUM(D13,G13)</f>
-        <v>96.694999999999993</v>
+        <v>53.839999999999996</v>
       </c>
       <c r="K13" s="18">
         <f>SUM(E13,H13)</f>
-        <v>-6.7000000000010829E-2</v>
+        <v>12.567000000000004</v>
       </c>
       <c r="L13" s="17">
         <f>I13-J13-K13</f>
-        <v>3.5527136788005009E-15</v>
+        <v>0</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>50</v>
@@ -7961,40 +7961,39 @@
       </c>
       <c r="B14" s="16">
         <f t="shared" ref="B14:B15" si="1">F14-C14</f>
-        <v>27.338999999999999</v>
+        <v>27.337</v>
       </c>
       <c r="C14" s="16">
-        <v>10.448</v>
+        <v>10.45</v>
       </c>
       <c r="D14" s="16">
-        <v>28.266999999999999</v>
+        <v>28.27</v>
       </c>
       <c r="E14" s="16">
         <f t="shared" ref="E14:E15" si="2">C14-D14</f>
-        <v>-17.818999999999999</v>
+        <v>-17.82</v>
       </c>
       <c r="F14" s="16">
         <v>37.786999999999999</v>
       </c>
       <c r="G14" s="16">
-        <f>F14-17.8</f>
-        <v>19.986999999999998</v>
+        <v>10.45</v>
       </c>
       <c r="H14" s="16">
         <f t="shared" ref="H14:H15" si="3">F14-G14</f>
-        <v>17.8</v>
+        <v>27.337</v>
       </c>
       <c r="I14" s="16">
         <f>SUM(C14,F14)</f>
-        <v>48.234999999999999</v>
+        <v>48.236999999999995</v>
       </c>
       <c r="J14" s="16">
         <f t="shared" si="0"/>
-        <v>48.253999999999998</v>
+        <v>38.72</v>
       </c>
       <c r="K14" s="18">
         <f>SUM(E14,H14)</f>
-        <v>-1.8999999999998352E-2</v>
+        <v>9.5169999999999995</v>
       </c>
       <c r="L14" s="17">
         <f>I14-J14-K14</f>
@@ -8012,40 +8011,39 @@
       </c>
       <c r="B15" s="16">
         <f t="shared" si="1"/>
-        <v>20.432999999999996</v>
+        <v>7.67</v>
       </c>
       <c r="C15" s="16">
-        <v>13.98</v>
+        <v>5.25</v>
       </c>
       <c r="D15" s="16">
-        <v>23.928000000000001</v>
+        <v>8.99</v>
       </c>
       <c r="E15" s="16">
         <f t="shared" si="2"/>
-        <v>-9.9480000000000004</v>
+        <v>-3.74</v>
       </c>
       <c r="F15" s="16">
-        <v>34.412999999999997</v>
+        <v>12.92</v>
       </c>
       <c r="G15" s="16">
-        <f>F15-9.9</f>
-        <v>24.512999999999998</v>
+        <v>6.13</v>
       </c>
       <c r="H15" s="16">
         <f t="shared" si="3"/>
-        <v>9.8999999999999986</v>
+        <v>6.79</v>
       </c>
       <c r="I15" s="16">
         <f>SUM(C15,F15)</f>
-        <v>48.393000000000001</v>
+        <v>18.170000000000002</v>
       </c>
       <c r="J15" s="16">
         <f t="shared" si="0"/>
-        <v>48.441000000000003</v>
+        <v>15.120000000000001</v>
       </c>
       <c r="K15" s="18">
         <f>SUM(E15,H15)</f>
-        <v>-4.8000000000001819E-2</v>
+        <v>3.05</v>
       </c>
       <c r="L15" s="17">
         <f>I15-J15-K15</f>
@@ -8058,6 +8056,7 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E16" s="16"/>
       <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -8327,7 +8326,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="22" t="s">
         <v>78</v>
       </c>
       <c r="I26" s="11"/>
@@ -8340,7 +8339,7 @@
       <c r="M26" s="15"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H27" s="22"/>
+      <c r="H27" s="23"/>
       <c r="I27" s="13">
         <f>SUM(I23:I25,I21,I18,I7)</f>
         <v>163.5</v>
@@ -8351,15 +8350,15 @@
       </c>
       <c r="K27" s="20">
         <f>SUM(K7,K10,K12,K13,K18,K21,K23,K24,K25)</f>
-        <v>-6.7000000000014381E-2</v>
+        <v>12.567</v>
       </c>
       <c r="L27" s="14">
         <f>I27-J27-K27</f>
-        <v>-0.93300000000001404</v>
+        <v>-13.567000000000029</v>
       </c>
       <c r="M27" s="15"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
       <c r="Q27" s="9"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -8371,8 +8370,8 @@
         <f>4.319+1.968</f>
         <v>6.2869999999999999</v>
       </c>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
       <c r="Q29" s="9"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -8380,8 +8379,8 @@
       <c r="Q30" s="6"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
       <c r="Q31" s="9"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -8389,8 +8388,8 @@
       <c r="Q32" s="6"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
       <c r="Q33" s="9"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -8398,8 +8397,8 @@
       <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
       <c r="Q35" s="9"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -8491,8 +8490,8 @@
       <c r="Q56" s="6"/>
     </row>
     <row r="57" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O57" s="24"/>
-      <c r="P57" s="24"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="21"/>
       <c r="Q57" s="9"/>
     </row>
     <row r="58" spans="15:17" x14ac:dyDescent="0.25">
@@ -8580,8 +8579,8 @@
       <c r="Q78" s="6"/>
     </row>
     <row r="79" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O79" s="24"/>
-      <c r="P79" s="24"/>
+      <c r="O79" s="21"/>
+      <c r="P79" s="21"/>
       <c r="Q79" s="9"/>
     </row>
     <row r="80" spans="15:17" x14ac:dyDescent="0.25">
@@ -8669,8 +8668,8 @@
       <c r="Q100" s="6"/>
     </row>
     <row r="101" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O101" s="24"/>
-      <c r="P101" s="24"/>
+      <c r="O101" s="21"/>
+      <c r="P101" s="21"/>
       <c r="Q101" s="9"/>
     </row>
     <row r="102" spans="15:17" x14ac:dyDescent="0.25">
@@ -8718,8 +8717,8 @@
       <c r="Q112" s="6"/>
     </row>
     <row r="113" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O113" s="24"/>
-      <c r="P113" s="24"/>
+      <c r="O113" s="21"/>
+      <c r="P113" s="21"/>
       <c r="Q113" s="9"/>
     </row>
     <row r="114" spans="15:17" x14ac:dyDescent="0.25">
@@ -8767,8 +8766,8 @@
       <c r="Q124" s="6"/>
     </row>
     <row r="125" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O125" s="24"/>
-      <c r="P125" s="24"/>
+      <c r="O125" s="21"/>
+      <c r="P125" s="21"/>
       <c r="Q125" s="9"/>
     </row>
     <row r="126" spans="15:17" x14ac:dyDescent="0.25">
@@ -8776,8 +8775,8 @@
       <c r="Q126" s="6"/>
     </row>
     <row r="127" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O127" s="24"/>
-      <c r="P127" s="24"/>
+      <c r="O127" s="21"/>
+      <c r="P127" s="21"/>
       <c r="Q127" s="9"/>
     </row>
     <row r="128" spans="15:17" x14ac:dyDescent="0.25">
@@ -8809,8 +8808,8 @@
       <c r="Q134" s="6"/>
     </row>
     <row r="135" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O135" s="24"/>
-      <c r="P135" s="24"/>
+      <c r="O135" s="21"/>
+      <c r="P135" s="21"/>
       <c r="Q135" s="9"/>
     </row>
     <row r="136" spans="15:17" x14ac:dyDescent="0.25">
@@ -8858,8 +8857,8 @@
       <c r="Q146" s="6"/>
     </row>
     <row r="147" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O147" s="24"/>
-      <c r="P147" s="24"/>
+      <c r="O147" s="21"/>
+      <c r="P147" s="21"/>
       <c r="Q147" s="9"/>
     </row>
     <row r="148" spans="15:17" x14ac:dyDescent="0.25">
@@ -8907,8 +8906,8 @@
       <c r="Q158" s="6"/>
     </row>
     <row r="159" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O159" s="24"/>
-      <c r="P159" s="24"/>
+      <c r="O159" s="21"/>
+      <c r="P159" s="21"/>
       <c r="Q159" s="9"/>
     </row>
     <row r="160" spans="15:17" x14ac:dyDescent="0.25">
@@ -8960,8 +8959,8 @@
       <c r="Q171" s="6"/>
     </row>
     <row r="172" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O172" s="24"/>
-      <c r="P172" s="24"/>
+      <c r="O172" s="21"/>
+      <c r="P172" s="21"/>
       <c r="Q172" s="9"/>
     </row>
     <row r="173" spans="15:17" x14ac:dyDescent="0.25">
@@ -9009,8 +9008,8 @@
       <c r="Q183" s="6"/>
     </row>
     <row r="184" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O184" s="24"/>
-      <c r="P184" s="24"/>
+      <c r="O184" s="21"/>
+      <c r="P184" s="21"/>
       <c r="Q184" s="9"/>
     </row>
     <row r="185" spans="15:17" x14ac:dyDescent="0.25">
@@ -9058,8 +9057,8 @@
       <c r="Q195" s="6"/>
     </row>
     <row r="196" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O196" s="24"/>
-      <c r="P196" s="24"/>
+      <c r="O196" s="21"/>
+      <c r="P196" s="21"/>
       <c r="Q196" s="9"/>
     </row>
     <row r="197" spans="15:17" x14ac:dyDescent="0.25">
@@ -9107,8 +9106,8 @@
       <c r="Q207" s="6"/>
     </row>
     <row r="208" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O208" s="24"/>
-      <c r="P208" s="24"/>
+      <c r="O208" s="21"/>
+      <c r="P208" s="21"/>
       <c r="Q208" s="9"/>
     </row>
     <row r="209" spans="15:17" x14ac:dyDescent="0.25">
@@ -9156,8 +9155,8 @@
       <c r="Q219" s="6"/>
     </row>
     <row r="220" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O220" s="24"/>
-      <c r="P220" s="24"/>
+      <c r="O220" s="21"/>
+      <c r="P220" s="21"/>
       <c r="Q220" s="9"/>
     </row>
     <row r="221" spans="15:17" x14ac:dyDescent="0.25">
@@ -9205,8 +9204,8 @@
       <c r="Q231" s="6"/>
     </row>
     <row r="232" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O232" s="24"/>
-      <c r="P232" s="24"/>
+      <c r="O232" s="21"/>
+      <c r="P232" s="21"/>
       <c r="Q232" s="9"/>
     </row>
     <row r="233" spans="15:17" x14ac:dyDescent="0.25">
@@ -9254,8 +9253,8 @@
       <c r="Q243" s="6"/>
     </row>
     <row r="244" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O244" s="24"/>
-      <c r="P244" s="24"/>
+      <c r="O244" s="21"/>
+      <c r="P244" s="21"/>
       <c r="Q244" s="9"/>
     </row>
     <row r="245" spans="15:17" x14ac:dyDescent="0.25">
@@ -9319,8 +9318,8 @@
       <c r="Q259" s="6"/>
     </row>
     <row r="260" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O260" s="24"/>
-      <c r="P260" s="24"/>
+      <c r="O260" s="21"/>
+      <c r="P260" s="21"/>
       <c r="Q260" s="9"/>
     </row>
     <row r="261" spans="15:17" x14ac:dyDescent="0.25">
@@ -9368,8 +9367,8 @@
       <c r="Q271" s="6"/>
     </row>
     <row r="272" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O272" s="24"/>
-      <c r="P272" s="24"/>
+      <c r="O272" s="21"/>
+      <c r="P272" s="21"/>
       <c r="Q272" s="9"/>
     </row>
     <row r="273" spans="15:17" x14ac:dyDescent="0.25">
@@ -9417,8 +9416,8 @@
       <c r="Q283" s="6"/>
     </row>
     <row r="284" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O284" s="24"/>
-      <c r="P284" s="24"/>
+      <c r="O284" s="21"/>
+      <c r="P284" s="21"/>
       <c r="Q284" s="9"/>
     </row>
     <row r="285" spans="15:17" x14ac:dyDescent="0.25">
@@ -9466,8 +9465,8 @@
       <c r="Q295" s="6"/>
     </row>
     <row r="296" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O296" s="24"/>
-      <c r="P296" s="24"/>
+      <c r="O296" s="21"/>
+      <c r="P296" s="21"/>
       <c r="Q296" s="9"/>
     </row>
     <row r="297" spans="15:17" x14ac:dyDescent="0.25">
@@ -9515,8 +9514,8 @@
       <c r="Q307" s="6"/>
     </row>
     <row r="308" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O308" s="24"/>
-      <c r="P308" s="24"/>
+      <c r="O308" s="21"/>
+      <c r="P308" s="21"/>
       <c r="Q308" s="9"/>
     </row>
     <row r="309" spans="15:17" x14ac:dyDescent="0.25">
@@ -9528,8 +9527,8 @@
       <c r="Q310" s="6"/>
     </row>
     <row r="311" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O311" s="24"/>
-      <c r="P311" s="24"/>
+      <c r="O311" s="21"/>
+      <c r="P311" s="21"/>
       <c r="Q311" s="9"/>
     </row>
     <row r="312" spans="15:17" x14ac:dyDescent="0.25">
@@ -9537,8 +9536,8 @@
       <c r="Q312" s="6"/>
     </row>
     <row r="313" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O313" s="24"/>
-      <c r="P313" s="24"/>
+      <c r="O313" s="21"/>
+      <c r="P313" s="21"/>
       <c r="Q313" s="9"/>
     </row>
     <row r="314" spans="15:17" x14ac:dyDescent="0.25">
@@ -9546,8 +9545,8 @@
       <c r="Q314" s="6"/>
     </row>
     <row r="315" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O315" s="24"/>
-      <c r="P315" s="24"/>
+      <c r="O315" s="21"/>
+      <c r="P315" s="21"/>
       <c r="Q315" s="9"/>
     </row>
     <row r="316" spans="15:17" x14ac:dyDescent="0.25">
@@ -9563,8 +9562,8 @@
       <c r="Q318" s="6"/>
     </row>
     <row r="319" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O319" s="24"/>
-      <c r="P319" s="24"/>
+      <c r="O319" s="21"/>
+      <c r="P319" s="21"/>
       <c r="Q319" s="9"/>
     </row>
     <row r="320" spans="15:17" x14ac:dyDescent="0.25">
@@ -9584,8 +9583,8 @@
       <c r="Q323" s="6"/>
     </row>
     <row r="324" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O324" s="24"/>
-      <c r="P324" s="24"/>
+      <c r="O324" s="21"/>
+      <c r="P324" s="21"/>
       <c r="Q324" s="9"/>
     </row>
     <row r="325" spans="15:17" x14ac:dyDescent="0.25">
@@ -9593,8 +9592,8 @@
       <c r="Q325" s="6"/>
     </row>
     <row r="326" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O326" s="24"/>
-      <c r="P326" s="24"/>
+      <c r="O326" s="21"/>
+      <c r="P326" s="21"/>
       <c r="Q326" s="9"/>
     </row>
     <row r="327" spans="15:17" x14ac:dyDescent="0.25">
@@ -9602,8 +9601,8 @@
       <c r="Q327" s="6"/>
     </row>
     <row r="328" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O328" s="24"/>
-      <c r="P328" s="24"/>
+      <c r="O328" s="21"/>
+      <c r="P328" s="21"/>
       <c r="Q328" s="9"/>
     </row>
     <row r="329" spans="15:17" x14ac:dyDescent="0.25">
@@ -9611,8 +9610,8 @@
       <c r="Q329" s="6"/>
     </row>
     <row r="330" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O330" s="24"/>
-      <c r="P330" s="24"/>
+      <c r="O330" s="21"/>
+      <c r="P330" s="21"/>
       <c r="Q330" s="9"/>
     </row>
     <row r="331" spans="15:17" x14ac:dyDescent="0.25">
@@ -9620,8 +9619,8 @@
       <c r="Q331" s="6"/>
     </row>
     <row r="332" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O332" s="24"/>
-      <c r="P332" s="24"/>
+      <c r="O332" s="21"/>
+      <c r="P332" s="21"/>
       <c r="Q332" s="9"/>
     </row>
     <row r="333" spans="15:17" x14ac:dyDescent="0.25">
@@ -9697,8 +9696,8 @@
       <c r="Q350" s="6"/>
     </row>
     <row r="351" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O351" s="24"/>
-      <c r="P351" s="24"/>
+      <c r="O351" s="21"/>
+      <c r="P351" s="21"/>
       <c r="Q351" s="9"/>
     </row>
     <row r="352" spans="15:17" x14ac:dyDescent="0.25">
@@ -9774,8 +9773,8 @@
       <c r="Q369" s="6"/>
     </row>
     <row r="370" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O370" s="24"/>
-      <c r="P370" s="24"/>
+      <c r="O370" s="21"/>
+      <c r="P370" s="21"/>
       <c r="Q370" s="9"/>
     </row>
     <row r="371" spans="15:17" x14ac:dyDescent="0.25">
@@ -9851,8 +9850,8 @@
       <c r="Q388" s="6"/>
     </row>
     <row r="389" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O389" s="24"/>
-      <c r="P389" s="24"/>
+      <c r="O389" s="21"/>
+      <c r="P389" s="21"/>
       <c r="Q389" s="9"/>
     </row>
     <row r="390" spans="15:17" x14ac:dyDescent="0.25">
@@ -9928,8 +9927,8 @@
       <c r="Q407" s="6"/>
     </row>
     <row r="408" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O408" s="24"/>
-      <c r="P408" s="24"/>
+      <c r="O408" s="21"/>
+      <c r="P408" s="21"/>
       <c r="Q408" s="9"/>
     </row>
     <row r="409" spans="15:17" x14ac:dyDescent="0.25">
@@ -10005,8 +10004,8 @@
       <c r="Q426" s="6"/>
     </row>
     <row r="427" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O427" s="24"/>
-      <c r="P427" s="24"/>
+      <c r="O427" s="21"/>
+      <c r="P427" s="21"/>
       <c r="Q427" s="9"/>
     </row>
     <row r="428" spans="15:17" x14ac:dyDescent="0.25">
@@ -10082,8 +10081,8 @@
       <c r="Q445" s="6"/>
     </row>
     <row r="446" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O446" s="24"/>
-      <c r="P446" s="24"/>
+      <c r="O446" s="21"/>
+      <c r="P446" s="21"/>
       <c r="Q446" s="9"/>
     </row>
     <row r="447" spans="15:17" x14ac:dyDescent="0.25">
@@ -10159,8 +10158,8 @@
       <c r="Q464" s="6"/>
     </row>
     <row r="465" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O465" s="24"/>
-      <c r="P465" s="24"/>
+      <c r="O465" s="21"/>
+      <c r="P465" s="21"/>
       <c r="Q465" s="9"/>
     </row>
     <row r="466" spans="15:17" x14ac:dyDescent="0.25">
@@ -10236,8 +10235,8 @@
       <c r="Q483" s="6"/>
     </row>
     <row r="484" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O484" s="24"/>
-      <c r="P484" s="24"/>
+      <c r="O484" s="21"/>
+      <c r="P484" s="21"/>
       <c r="Q484" s="9"/>
     </row>
     <row r="485" spans="15:17" x14ac:dyDescent="0.25">
@@ -10325,8 +10324,8 @@
       <c r="Q505" s="6"/>
     </row>
     <row r="506" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O506" s="24"/>
-      <c r="P506" s="24"/>
+      <c r="O506" s="21"/>
+      <c r="P506" s="21"/>
       <c r="Q506" s="9"/>
     </row>
     <row r="507" spans="15:17" x14ac:dyDescent="0.25">
@@ -10402,8 +10401,8 @@
       <c r="Q524" s="6"/>
     </row>
     <row r="525" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O525" s="24"/>
-      <c r="P525" s="24"/>
+      <c r="O525" s="21"/>
+      <c r="P525" s="21"/>
       <c r="Q525" s="9"/>
     </row>
     <row r="526" spans="15:17" x14ac:dyDescent="0.25">
@@ -10479,8 +10478,8 @@
       <c r="Q543" s="6"/>
     </row>
     <row r="544" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O544" s="24"/>
-      <c r="P544" s="24"/>
+      <c r="O544" s="21"/>
+      <c r="P544" s="21"/>
       <c r="Q544" s="9"/>
     </row>
     <row r="545" spans="15:17" x14ac:dyDescent="0.25">
@@ -10556,8 +10555,8 @@
       <c r="Q562" s="6"/>
     </row>
     <row r="563" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O563" s="24"/>
-      <c r="P563" s="24"/>
+      <c r="O563" s="21"/>
+      <c r="P563" s="21"/>
       <c r="Q563" s="9"/>
     </row>
     <row r="564" spans="15:17" x14ac:dyDescent="0.25">
@@ -10633,8 +10632,8 @@
       <c r="Q581" s="6"/>
     </row>
     <row r="582" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O582" s="24"/>
-      <c r="P582" s="24"/>
+      <c r="O582" s="21"/>
+      <c r="P582" s="21"/>
       <c r="Q582" s="9"/>
     </row>
     <row r="583" spans="15:17" x14ac:dyDescent="0.25">
@@ -10670,8 +10669,8 @@
       <c r="Q590" s="6"/>
     </row>
     <row r="591" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O591" s="24"/>
-      <c r="P591" s="24"/>
+      <c r="O591" s="21"/>
+      <c r="P591" s="21"/>
       <c r="Q591" s="9"/>
     </row>
     <row r="592" spans="15:17" x14ac:dyDescent="0.25">
@@ -10679,8 +10678,8 @@
       <c r="Q592" s="6"/>
     </row>
     <row r="593" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O593" s="24"/>
-      <c r="P593" s="24"/>
+      <c r="O593" s="21"/>
+      <c r="P593" s="21"/>
       <c r="Q593" s="9"/>
     </row>
     <row r="594" spans="15:17" x14ac:dyDescent="0.25">
@@ -10692,8 +10691,8 @@
       <c r="Q595" s="6"/>
     </row>
     <row r="596" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O596" s="24"/>
-      <c r="P596" s="24"/>
+      <c r="O596" s="21"/>
+      <c r="P596" s="21"/>
       <c r="Q596" s="9"/>
     </row>
     <row r="597" spans="15:17" x14ac:dyDescent="0.25">
@@ -10701,8 +10700,8 @@
       <c r="Q597" s="6"/>
     </row>
     <row r="598" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O598" s="24"/>
-      <c r="P598" s="24"/>
+      <c r="O598" s="21"/>
+      <c r="P598" s="21"/>
       <c r="Q598" s="9"/>
     </row>
     <row r="599" spans="15:17" x14ac:dyDescent="0.25">
@@ -10782,8 +10781,8 @@
       <c r="Q617" s="6"/>
     </row>
     <row r="618" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O618" s="24"/>
-      <c r="P618" s="24"/>
+      <c r="O618" s="21"/>
+      <c r="P618" s="21"/>
       <c r="Q618" s="9"/>
     </row>
     <row r="619" spans="15:17" x14ac:dyDescent="0.25">
@@ -10823,8 +10822,8 @@
       <c r="Q627" s="6"/>
     </row>
     <row r="628" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O628" s="24"/>
-      <c r="P628" s="24"/>
+      <c r="O628" s="21"/>
+      <c r="P628" s="21"/>
       <c r="Q628" s="9"/>
     </row>
     <row r="629" spans="15:17" x14ac:dyDescent="0.25">
@@ -10888,8 +10887,8 @@
       <c r="Q643" s="6"/>
     </row>
     <row r="644" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O644" s="24"/>
-      <c r="P644" s="24"/>
+      <c r="O644" s="21"/>
+      <c r="P644" s="21"/>
       <c r="Q644" s="9"/>
     </row>
     <row r="645" spans="15:17" x14ac:dyDescent="0.25">
@@ -10913,8 +10912,8 @@
       <c r="Q649" s="6"/>
     </row>
     <row r="650" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O650" s="24"/>
-      <c r="P650" s="24"/>
+      <c r="O650" s="21"/>
+      <c r="P650" s="21"/>
       <c r="Q650" s="9"/>
     </row>
     <row r="651" spans="15:17" x14ac:dyDescent="0.25">
@@ -10922,8 +10921,8 @@
       <c r="Q651" s="6"/>
     </row>
     <row r="652" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O652" s="24"/>
-      <c r="P652" s="24"/>
+      <c r="O652" s="21"/>
+      <c r="P652" s="21"/>
       <c r="Q652" s="9"/>
     </row>
     <row r="653" spans="15:17" x14ac:dyDescent="0.25">
@@ -10931,8 +10930,8 @@
       <c r="Q653" s="6"/>
     </row>
     <row r="654" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O654" s="24"/>
-      <c r="P654" s="24"/>
+      <c r="O654" s="21"/>
+      <c r="P654" s="21"/>
       <c r="Q654" s="9"/>
     </row>
     <row r="655" spans="15:17" x14ac:dyDescent="0.25">
@@ -10940,8 +10939,8 @@
       <c r="Q655" s="6"/>
     </row>
     <row r="656" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O656" s="24"/>
-      <c r="P656" s="24"/>
+      <c r="O656" s="21"/>
+      <c r="P656" s="21"/>
       <c r="Q656" s="9"/>
     </row>
     <row r="657" spans="15:17" x14ac:dyDescent="0.25">
@@ -10949,8 +10948,8 @@
       <c r="Q657" s="6"/>
     </row>
     <row r="658" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O658" s="24"/>
-      <c r="P658" s="24"/>
+      <c r="O658" s="21"/>
+      <c r="P658" s="21"/>
       <c r="Q658" s="9"/>
     </row>
     <row r="659" spans="15:17" x14ac:dyDescent="0.25">
@@ -10958,8 +10957,8 @@
       <c r="Q659" s="6"/>
     </row>
     <row r="660" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O660" s="24"/>
-      <c r="P660" s="24"/>
+      <c r="O660" s="21"/>
+      <c r="P660" s="21"/>
       <c r="Q660" s="9"/>
     </row>
     <row r="661" spans="15:17" x14ac:dyDescent="0.25">
@@ -10967,8 +10966,8 @@
       <c r="Q661" s="6"/>
     </row>
     <row r="662" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O662" s="24"/>
-      <c r="P662" s="24"/>
+      <c r="O662" s="21"/>
+      <c r="P662" s="21"/>
       <c r="Q662" s="9"/>
     </row>
     <row r="663" spans="15:17" x14ac:dyDescent="0.25">
@@ -10976,8 +10975,8 @@
       <c r="Q663" s="6"/>
     </row>
     <row r="664" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O664" s="24"/>
-      <c r="P664" s="24"/>
+      <c r="O664" s="21"/>
+      <c r="P664" s="21"/>
       <c r="Q664" s="9"/>
     </row>
     <row r="665" spans="15:17" x14ac:dyDescent="0.25">
@@ -10985,8 +10984,8 @@
       <c r="Q665" s="6"/>
     </row>
     <row r="666" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O666" s="24"/>
-      <c r="P666" s="24"/>
+      <c r="O666" s="21"/>
+      <c r="P666" s="21"/>
       <c r="Q666" s="9"/>
     </row>
     <row r="667" spans="15:17" x14ac:dyDescent="0.25">
@@ -10994,8 +10993,8 @@
       <c r="Q667" s="6"/>
     </row>
     <row r="668" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O668" s="24"/>
-      <c r="P668" s="24"/>
+      <c r="O668" s="21"/>
+      <c r="P668" s="21"/>
       <c r="Q668" s="9"/>
     </row>
     <row r="669" spans="15:17" x14ac:dyDescent="0.25">
@@ -11003,8 +11002,8 @@
       <c r="Q669" s="6"/>
     </row>
     <row r="670" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O670" s="24"/>
-      <c r="P670" s="24"/>
+      <c r="O670" s="21"/>
+      <c r="P670" s="21"/>
       <c r="Q670" s="9"/>
     </row>
     <row r="671" spans="15:17" x14ac:dyDescent="0.25">
@@ -11012,8 +11011,8 @@
       <c r="Q671" s="6"/>
     </row>
     <row r="672" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O672" s="24"/>
-      <c r="P672" s="24"/>
+      <c r="O672" s="21"/>
+      <c r="P672" s="21"/>
       <c r="Q672" s="9"/>
     </row>
     <row r="673" spans="15:17" x14ac:dyDescent="0.25">
@@ -11021,8 +11020,8 @@
       <c r="Q673" s="6"/>
     </row>
     <row r="674" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O674" s="24"/>
-      <c r="P674" s="24"/>
+      <c r="O674" s="21"/>
+      <c r="P674" s="21"/>
       <c r="Q674" s="9"/>
     </row>
     <row r="675" spans="15:17" x14ac:dyDescent="0.25">
@@ -11030,8 +11029,8 @@
       <c r="Q675" s="6"/>
     </row>
     <row r="676" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O676" s="24"/>
-      <c r="P676" s="24"/>
+      <c r="O676" s="21"/>
+      <c r="P676" s="21"/>
       <c r="Q676" s="9"/>
     </row>
     <row r="677" spans="15:17" x14ac:dyDescent="0.25">
@@ -11039,8 +11038,8 @@
       <c r="Q677" s="6"/>
     </row>
     <row r="678" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O678" s="24"/>
-      <c r="P678" s="24"/>
+      <c r="O678" s="21"/>
+      <c r="P678" s="21"/>
       <c r="Q678" s="9"/>
     </row>
     <row r="679" spans="15:17" x14ac:dyDescent="0.25">
@@ -11072,8 +11071,8 @@
       <c r="Q685" s="6"/>
     </row>
     <row r="686" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O686" s="24"/>
-      <c r="P686" s="24"/>
+      <c r="O686" s="21"/>
+      <c r="P686" s="21"/>
       <c r="Q686" s="9"/>
     </row>
     <row r="687" spans="15:17" x14ac:dyDescent="0.25">
@@ -11081,8 +11080,8 @@
       <c r="Q687" s="6"/>
     </row>
     <row r="688" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O688" s="24"/>
-      <c r="P688" s="24"/>
+      <c r="O688" s="21"/>
+      <c r="P688" s="21"/>
       <c r="Q688" s="9"/>
     </row>
     <row r="689" spans="15:17" x14ac:dyDescent="0.25">
@@ -11094,6 +11093,66 @@
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="O686:P686"/>
+    <mergeCell ref="O666:P666"/>
+    <mergeCell ref="O618:P618"/>
+    <mergeCell ref="O628:P628"/>
+    <mergeCell ref="O644:P644"/>
+    <mergeCell ref="O650:P650"/>
+    <mergeCell ref="O652:P652"/>
+    <mergeCell ref="O654:P654"/>
+    <mergeCell ref="O656:P656"/>
+    <mergeCell ref="O658:P658"/>
+    <mergeCell ref="O660:P660"/>
+    <mergeCell ref="O662:P662"/>
+    <mergeCell ref="O688:P688"/>
+    <mergeCell ref="O668:P668"/>
+    <mergeCell ref="O670:P670"/>
+    <mergeCell ref="O672:P672"/>
+    <mergeCell ref="O674:P674"/>
+    <mergeCell ref="O676:P676"/>
+    <mergeCell ref="O678:P678"/>
+    <mergeCell ref="O664:P664"/>
+    <mergeCell ref="O598:P598"/>
+    <mergeCell ref="O446:P446"/>
+    <mergeCell ref="O465:P465"/>
+    <mergeCell ref="O484:P484"/>
+    <mergeCell ref="O506:P506"/>
+    <mergeCell ref="O525:P525"/>
+    <mergeCell ref="O544:P544"/>
+    <mergeCell ref="O563:P563"/>
+    <mergeCell ref="O582:P582"/>
+    <mergeCell ref="O591:P591"/>
+    <mergeCell ref="O593:P593"/>
+    <mergeCell ref="O596:P596"/>
+    <mergeCell ref="O427:P427"/>
+    <mergeCell ref="O315:P315"/>
+    <mergeCell ref="O319:P319"/>
+    <mergeCell ref="O324:P324"/>
+    <mergeCell ref="O326:P326"/>
+    <mergeCell ref="O328:P328"/>
+    <mergeCell ref="O330:P330"/>
+    <mergeCell ref="O332:P332"/>
+    <mergeCell ref="O351:P351"/>
+    <mergeCell ref="O370:P370"/>
+    <mergeCell ref="O389:P389"/>
+    <mergeCell ref="O408:P408"/>
+    <mergeCell ref="O313:P313"/>
+    <mergeCell ref="O196:P196"/>
+    <mergeCell ref="O208:P208"/>
+    <mergeCell ref="O220:P220"/>
+    <mergeCell ref="O232:P232"/>
+    <mergeCell ref="O244:P244"/>
+    <mergeCell ref="O260:P260"/>
+    <mergeCell ref="O272:P272"/>
+    <mergeCell ref="O284:P284"/>
+    <mergeCell ref="O296:P296"/>
+    <mergeCell ref="O308:P308"/>
+    <mergeCell ref="O311:P311"/>
     <mergeCell ref="O33:P33"/>
     <mergeCell ref="O27:P27"/>
     <mergeCell ref="O29:P29"/>
@@ -11110,66 +11169,6 @@
     <mergeCell ref="O147:P147"/>
     <mergeCell ref="O159:P159"/>
     <mergeCell ref="O172:P172"/>
-    <mergeCell ref="O313:P313"/>
-    <mergeCell ref="O196:P196"/>
-    <mergeCell ref="O208:P208"/>
-    <mergeCell ref="O220:P220"/>
-    <mergeCell ref="O232:P232"/>
-    <mergeCell ref="O244:P244"/>
-    <mergeCell ref="O260:P260"/>
-    <mergeCell ref="O272:P272"/>
-    <mergeCell ref="O284:P284"/>
-    <mergeCell ref="O296:P296"/>
-    <mergeCell ref="O308:P308"/>
-    <mergeCell ref="O311:P311"/>
-    <mergeCell ref="O427:P427"/>
-    <mergeCell ref="O315:P315"/>
-    <mergeCell ref="O319:P319"/>
-    <mergeCell ref="O324:P324"/>
-    <mergeCell ref="O326:P326"/>
-    <mergeCell ref="O328:P328"/>
-    <mergeCell ref="O330:P330"/>
-    <mergeCell ref="O332:P332"/>
-    <mergeCell ref="O351:P351"/>
-    <mergeCell ref="O370:P370"/>
-    <mergeCell ref="O389:P389"/>
-    <mergeCell ref="O408:P408"/>
-    <mergeCell ref="O664:P664"/>
-    <mergeCell ref="O598:P598"/>
-    <mergeCell ref="O446:P446"/>
-    <mergeCell ref="O465:P465"/>
-    <mergeCell ref="O484:P484"/>
-    <mergeCell ref="O506:P506"/>
-    <mergeCell ref="O525:P525"/>
-    <mergeCell ref="O544:P544"/>
-    <mergeCell ref="O563:P563"/>
-    <mergeCell ref="O582:P582"/>
-    <mergeCell ref="O591:P591"/>
-    <mergeCell ref="O593:P593"/>
-    <mergeCell ref="O596:P596"/>
-    <mergeCell ref="O688:P688"/>
-    <mergeCell ref="O668:P668"/>
-    <mergeCell ref="O670:P670"/>
-    <mergeCell ref="O672:P672"/>
-    <mergeCell ref="O674:P674"/>
-    <mergeCell ref="O676:P676"/>
-    <mergeCell ref="O678:P678"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="O686:P686"/>
-    <mergeCell ref="O666:P666"/>
-    <mergeCell ref="O618:P618"/>
-    <mergeCell ref="O628:P628"/>
-    <mergeCell ref="O644:P644"/>
-    <mergeCell ref="O650:P650"/>
-    <mergeCell ref="O652:P652"/>
-    <mergeCell ref="O654:P654"/>
-    <mergeCell ref="O656:P656"/>
-    <mergeCell ref="O658:P658"/>
-    <mergeCell ref="O660:P660"/>
-    <mergeCell ref="O662:P662"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>